<commit_message>
Checking in Event config
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDriver/TestIFRS9/Test.xlsx
+++ b/src/test/resources/TestDriver/TestIFRS9/Test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arahmed\OneDrive - SS&amp;C Technologies, Inc\Desktop\Pers\IFRS9_Collateral\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arahmed\OneDrive - SS&amp;C Technologies, Inc\Desktop\Pers\IFRS9_Collateral\TestIFRS9\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99AB4963-610C-48C7-B10B-80F4B8BCD1D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29CE352B-5997-4828-A252-EEBEE0CADE86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2505" yWindow="2670" windowWidth="21600" windowHeight="11295" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="1" r:id="rId1"/>
@@ -169,9 +169,6 @@
     <t>TestIFRS9/ActivityDataD2.xlsx</t>
   </si>
   <si>
-    <t>TestIFRS9/EventConfigurations.jL00n</t>
-  </si>
-  <si>
     <t>{"instrumentId": "L001"}</t>
   </si>
   <si>
@@ -206,6 +203,9 @@
   </si>
   <si>
     <t>L006</t>
+  </si>
+  <si>
+    <t>TestIFRS9/EventConfigurations.json</t>
   </si>
 </sst>
 </file>
@@ -511,8 +511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -553,7 +553,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -654,7 +654,7 @@
         <v>28</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -682,10 +682,10 @@
         <v>20240930</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3">
         <v>437.89499999999998</v>
@@ -703,10 +703,10 @@
         <v>20241231</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4" s="11">
         <v>-73.215900000000033</v>
@@ -752,7 +752,7 @@
         <v>28</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -780,10 +780,10 @@
         <v>20240930</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D3">
         <v>437854.35</v>
@@ -801,10 +801,10 @@
         <v>20241231</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D4" s="8">
         <v>-5671.234999999986</v>
@@ -874,7 +874,7 @@
         <v>20240930</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" s="1">
         <v>0</v>
@@ -893,7 +893,7 @@
         <v>20241231</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" s="1">
         <f>E3</f>
@@ -941,7 +941,7 @@
         <v>13</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G1" s="5"/>
     </row>
@@ -956,7 +956,7 @@
         <v>16</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>17</v>
@@ -985,7 +985,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>23</v>
@@ -994,7 +994,7 @@
         <v>20240930</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G3">
         <v>829.61659999999995</v>
@@ -1017,7 +1017,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>23</v>
@@ -1026,7 +1026,7 @@
         <v>20241231</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G4" s="8">
         <v>-72.746099999999956</v>
@@ -1080,7 +1080,7 @@
         <v>28</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1108,10 +1108,10 @@
         <v>20240930</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D3" s="14">
         <v>829.61659999999995</v>
@@ -1128,10 +1128,10 @@
         <v>20241231</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D4" s="8">
         <v>-72.746099999999956</v>
@@ -1178,7 +1178,7 @@
         <v>13</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G1" s="5"/>
     </row>
@@ -1193,7 +1193,7 @@
         <v>16</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>17</v>
@@ -1222,7 +1222,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>23</v>
@@ -1231,7 +1231,7 @@
         <v>20240930</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G3">
         <v>16127.9249</v>
@@ -1254,7 +1254,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>23</v>
@@ -1263,7 +1263,7 @@
         <v>20241231</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G4" s="8">
         <v>-426.63560000000143</v>
@@ -1310,7 +1310,7 @@
         <v>28</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1338,10 +1338,10 @@
         <v>20240930</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" s="12">
         <v>16127.9249</v>
@@ -1359,10 +1359,10 @@
         <v>20241231</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D4" s="12">
         <v>-426.63560000000143</v>
@@ -1405,7 +1405,7 @@
         <v>13</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G1" s="5"/>
     </row>
@@ -1420,7 +1420,7 @@
         <v>16</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>17</v>
@@ -1449,7 +1449,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>23</v>
@@ -1458,7 +1458,7 @@
         <v>20240930</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G3" s="11">
         <v>945.57389999999998</v>
@@ -1481,7 +1481,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>23</v>
@@ -1490,7 +1490,7 @@
         <v>20241231</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G4" s="11">
         <v>-537.53749999999991</v>
@@ -1534,7 +1534,7 @@
         <v>13</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G1" s="5"/>
     </row>
@@ -1549,7 +1549,7 @@
         <v>16</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>17</v>
@@ -1578,7 +1578,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>23</v>
@@ -1587,7 +1587,7 @@
         <v>20240930</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G3">
         <v>437.89499999999998</v>
@@ -1610,7 +1610,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>23</v>
@@ -1619,7 +1619,7 @@
         <v>20241231</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G4" s="11">
         <v>-73.215900000000033</v>
@@ -1648,7 +1648,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CB707A6-16AA-42D5-BBFE-93ACD3FDBA16}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -1663,7 +1663,7 @@
         <v>13</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G1" s="5"/>
     </row>
@@ -1678,7 +1678,7 @@
         <v>16</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>17</v>
@@ -1707,7 +1707,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>23</v>
@@ -1716,7 +1716,7 @@
         <v>20240930</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G3">
         <v>437854.35</v>
@@ -1739,7 +1739,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>23</v>
@@ -1748,7 +1748,7 @@
         <v>20241231</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G4" s="8">
         <v>-5671.234999999986</v>
@@ -1795,7 +1795,7 @@
         <v>28</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1823,10 +1823,10 @@
         <v>20240930</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D3" s="12">
         <v>945.57389999999998</v>
@@ -1844,10 +1844,10 @@
         <v>20241231</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D4" s="12">
         <v>-537.53749999999991</v>

</xml_diff>

<commit_message>
Checking in ifrs9 output
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDriver/TestIFRS9/Test.xlsx
+++ b/src/test/resources/TestDriver/TestIFRS9/Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arahmed\OneDrive - SS&amp;C Technologies, Inc\Desktop\Pers\IFRS9_Collateral\TestIFRS9\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29CE352B-5997-4828-A252-EEBEE0CADE86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A9592C5-C4AC-4610-8824-2D931D0A30D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2505" yWindow="2670" windowWidth="21600" windowHeight="11295" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="1" r:id="rId1"/>
@@ -172,9 +172,6 @@
     <t>{"instrumentId": "L001"}</t>
   </si>
   <si>
-    <t>L00urce ASC</t>
-  </si>
-  <si>
     <t>L001</t>
   </si>
   <si>
@@ -206,6 +203,9 @@
   </si>
   <si>
     <t>TestIFRS9/EventConfigurations.json</t>
+  </si>
+  <si>
+    <t>Source ASC</t>
   </si>
 </sst>
 </file>
@@ -511,7 +511,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -553,7 +553,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -654,7 +654,7 @@
         <v>28</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -682,10 +682,10 @@
         <v>20240930</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D3">
         <v>437.89499999999998</v>
@@ -703,10 +703,10 @@
         <v>20241231</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4" s="11">
         <v>-73.215900000000033</v>
@@ -752,7 +752,7 @@
         <v>28</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -780,10 +780,10 @@
         <v>20240930</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D3">
         <v>437854.35</v>
@@ -801,10 +801,10 @@
         <v>20241231</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D4" s="8">
         <v>-5671.234999999986</v>
@@ -832,7 +832,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -874,7 +876,7 @@
         <v>20240930</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" s="1">
         <v>0</v>
@@ -893,7 +895,7 @@
         <v>20241231</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" s="1">
         <f>E3</f>
@@ -926,8 +928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:G4"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -956,7 +958,7 @@
         <v>16</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>17</v>
@@ -985,7 +987,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>23</v>
@@ -994,7 +996,7 @@
         <v>20240930</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G3">
         <v>829.61659999999995</v>
@@ -1017,7 +1019,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>23</v>
@@ -1026,7 +1028,7 @@
         <v>20241231</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G4" s="8">
         <v>-72.746099999999956</v>
@@ -1108,10 +1110,10 @@
         <v>20240930</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D3" s="14">
         <v>829.61659999999995</v>
@@ -1128,10 +1130,10 @@
         <v>20241231</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D4" s="8">
         <v>-72.746099999999956</v>
@@ -1164,7 +1166,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:G4"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1178,7 +1180,7 @@
         <v>13</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G1" s="5"/>
     </row>
@@ -1193,7 +1195,7 @@
         <v>16</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>17</v>
@@ -1222,7 +1224,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>23</v>
@@ -1231,7 +1233,7 @@
         <v>20240930</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G3">
         <v>16127.9249</v>
@@ -1254,7 +1256,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>23</v>
@@ -1263,7 +1265,7 @@
         <v>20241231</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G4" s="8">
         <v>-426.63560000000143</v>
@@ -1310,7 +1312,7 @@
         <v>28</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1338,10 +1340,10 @@
         <v>20240930</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D3" s="12">
         <v>16127.9249</v>
@@ -1359,10 +1361,10 @@
         <v>20241231</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D4" s="12">
         <v>-426.63560000000143</v>
@@ -1391,7 +1393,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:G4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1405,7 +1407,7 @@
         <v>13</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G1" s="5"/>
     </row>
@@ -1420,7 +1422,7 @@
         <v>16</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>17</v>
@@ -1449,7 +1451,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>23</v>
@@ -1458,7 +1460,7 @@
         <v>20240930</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G3" s="11">
         <v>945.57389999999998</v>
@@ -1481,7 +1483,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>23</v>
@@ -1490,7 +1492,7 @@
         <v>20241231</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G4" s="11">
         <v>-537.53749999999991</v>
@@ -1520,7 +1522,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:G4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1534,7 +1536,7 @@
         <v>13</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G1" s="5"/>
     </row>
@@ -1549,7 +1551,7 @@
         <v>16</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>17</v>
@@ -1578,7 +1580,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>23</v>
@@ -1587,7 +1589,7 @@
         <v>20240930</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G3">
         <v>437.89499999999998</v>
@@ -1610,7 +1612,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>23</v>
@@ -1619,7 +1621,7 @@
         <v>20241231</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G4" s="11">
         <v>-73.215900000000033</v>
@@ -1649,7 +1651,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1663,7 +1665,7 @@
         <v>13</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G1" s="5"/>
     </row>
@@ -1678,7 +1680,7 @@
         <v>16</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>17</v>
@@ -1707,7 +1709,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>23</v>
@@ -1716,7 +1718,7 @@
         <v>20240930</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G3">
         <v>437854.35</v>
@@ -1739,7 +1741,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>23</v>
@@ -1748,7 +1750,7 @@
         <v>20241231</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G4" s="8">
         <v>-5671.234999999986</v>
@@ -1795,7 +1797,7 @@
         <v>28</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1823,10 +1825,10 @@
         <v>20240930</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D3" s="12">
         <v>945.57389999999998</v>
@@ -1844,10 +1846,10 @@
         <v>20241231</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D4" s="12">
         <v>-537.53749999999991</v>

</xml_diff>

<commit_message>
Updating Output for IFRS9 case
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDriver/TestIFRS9/Test.xlsx
+++ b/src/test/resources/TestDriver/TestIFRS9/Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arahmed\OneDrive - SS&amp;C Technologies, Inc\Desktop\Pers\IFRS9_Collateral\TestIFRS9\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A9592C5-C4AC-4610-8824-2D931D0A30D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E81C06-C259-4D87-A787-D58DAF98AB81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="1" r:id="rId1"/>
@@ -295,7 +295,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -313,6 +313,7 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -637,7 +638,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -688,14 +689,15 @@
         <v>43</v>
       </c>
       <c r="D3">
-        <v>437.89499999999998</v>
-      </c>
-      <c r="E3" s="12">
+        <f>O_TransactionActivity3!G3</f>
+        <v>945.57389999999998</v>
+      </c>
+      <c r="E3" s="9">
         <v>0</v>
       </c>
-      <c r="F3" s="12">
-        <f>D3</f>
-        <v>437.89499999999998</v>
+      <c r="F3" s="15">
+        <f>D3+E3</f>
+        <v>945.57389999999998</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -708,16 +710,17 @@
       <c r="C4" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="11">
-        <v>-73.215900000000033</v>
-      </c>
-      <c r="E4" s="12">
+      <c r="D4">
+        <f>O_TransactionActivity3!G4</f>
+        <v>-537.53749999999991</v>
+      </c>
+      <c r="E4" s="14">
         <f>F3</f>
-        <v>437.89499999999998</v>
-      </c>
-      <c r="F4" s="12">
-        <f>E4+D4</f>
-        <v>364.67909999999995</v>
+        <v>945.57389999999998</v>
+      </c>
+      <c r="F4" s="15">
+        <f>D4+E4</f>
+        <v>408.03640000000007</v>
       </c>
     </row>
   </sheetData>
@@ -735,7 +738,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -786,14 +789,15 @@
         <v>46</v>
       </c>
       <c r="D3">
-        <v>437854.35</v>
-      </c>
-      <c r="E3" s="12">
+        <f>O_TransactionActivity6!G3</f>
+        <v>437854.35000000003</v>
+      </c>
+      <c r="E3" s="9">
         <v>0</v>
       </c>
-      <c r="F3" s="12">
-        <f>D3</f>
-        <v>437854.35</v>
+      <c r="F3" s="15">
+        <f>D3+E3</f>
+        <v>437854.35000000003</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -807,14 +811,15 @@
         <v>46</v>
       </c>
       <c r="D4" s="8">
-        <v>-5671.234999999986</v>
-      </c>
-      <c r="E4" s="12">
+        <f>O_TransactionActivity6!G4</f>
+        <v>-5671.2350000000442</v>
+      </c>
+      <c r="E4" s="14">
         <f>F3</f>
-        <v>437854.35</v>
-      </c>
-      <c r="F4" s="12">
-        <f>E4+D4</f>
+        <v>437854.35000000003</v>
+      </c>
+      <c r="F4" s="15">
+        <f>D4+E4</f>
         <v>432183.11499999999</v>
       </c>
     </row>
@@ -832,8 +837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -882,12 +887,12 @@
         <v>0</v>
       </c>
       <c r="D3" s="1">
-        <f>O_TransactionActivity!G3+O_TransactionActivity2!G3+O_TransactionActivity3!G3+O_TransactionActivity5!G3+O_TransactionActivity6!G3</f>
-        <v>456195.36040000001</v>
+        <f>O_TransactionActivity6!G3+O_TransactionActivity5!G3+O_TransactionActivity3!G3+O_TransactionActivity2!G3+O_TransactionActivity!G3</f>
+        <v>456205.4740000001</v>
       </c>
       <c r="E3" s="1">
-        <f>D3</f>
-        <v>456195.36040000001</v>
+        <f>C3+D3</f>
+        <v>456205.4740000001</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -899,15 +904,15 @@
       </c>
       <c r="C4" s="1">
         <f>E3</f>
-        <v>456195.36040000001</v>
+        <v>456205.4740000001</v>
       </c>
       <c r="D4" s="1">
-        <f>O_TransactionActivity!G4+O_TransactionActivity2!G4+O_TransactionActivity3!G4+O_TransactionActivity5!G4+O_TransactionActivity6!G4</f>
-        <v>-6781.3700999999874</v>
+        <f>O_TransactionActivity6!G4+O_TransactionActivity5!G4+O_TransactionActivity3!G4+O_TransactionActivity2!G4+O_TransactionActivity!G4</f>
+        <v>-6791.4837000000452</v>
       </c>
       <c r="E4" s="1">
         <f>C4+D4</f>
-        <v>449413.9903</v>
+        <v>449413.99030000006</v>
       </c>
     </row>
   </sheetData>
@@ -928,8 +933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -999,7 +1004,7 @@
         <v>37</v>
       </c>
       <c r="G3">
-        <v>829.61659999999995</v>
+        <v>830.10309999999993</v>
       </c>
       <c r="H3" s="7">
         <v>202409</v>
@@ -1031,7 +1036,7 @@
         <v>37</v>
       </c>
       <c r="G4" s="8">
-        <v>-72.746099999999956</v>
+        <v>-73.232599999999934</v>
       </c>
       <c r="H4" s="7">
         <v>202412</v>
@@ -1065,7 +1070,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F4"/>
+      <selection activeCell="E3" sqref="E3:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1116,13 +1121,15 @@
         <v>37</v>
       </c>
       <c r="D3" s="14">
-        <v>829.61659999999995</v>
+        <f>O_TransactionActivity!G3</f>
+        <v>830.10309999999993</v>
       </c>
       <c r="E3" s="9">
         <v>0</v>
       </c>
-      <c r="F3" s="14">
-        <v>829.61659999999995</v>
+      <c r="F3" s="15">
+        <f>D3+E3</f>
+        <v>830.10309999999993</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1135,14 +1142,16 @@
       <c r="C4" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="8">
-        <v>-72.746099999999956</v>
+      <c r="D4" s="14">
+        <f>O_TransactionActivity!G4</f>
+        <v>-73.232599999999934</v>
       </c>
       <c r="E4" s="14">
-        <v>829.61659999999995</v>
-      </c>
-      <c r="F4" s="9">
-        <f>E4+D4</f>
+        <f>F3</f>
+        <v>830.10309999999993</v>
+      </c>
+      <c r="F4" s="15">
+        <f>D4+E4</f>
         <v>756.87049999999999</v>
       </c>
     </row>
@@ -1166,7 +1175,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1236,7 +1245,7 @@
         <v>39</v>
       </c>
       <c r="G3">
-        <v>16127.9249</v>
+        <v>16137.294699999999</v>
       </c>
       <c r="H3" s="7">
         <v>202409</v>
@@ -1268,7 +1277,7 @@
         <v>39</v>
       </c>
       <c r="G4" s="8">
-        <v>-426.63560000000143</v>
+        <v>-436.00540000000001</v>
       </c>
       <c r="H4" s="7">
         <v>202412</v>
@@ -1295,7 +1304,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1346,14 +1355,15 @@
         <v>39</v>
       </c>
       <c r="D3" s="12">
-        <v>16127.9249</v>
-      </c>
-      <c r="E3" s="12">
+        <f>O_TransactionActivity2!G3</f>
+        <v>16137.294699999999</v>
+      </c>
+      <c r="E3" s="9">
         <v>0</v>
       </c>
-      <c r="F3" s="12">
-        <f>D3</f>
-        <v>16127.9249</v>
+      <c r="F3" s="15">
+        <f>D3+E3</f>
+        <v>16137.294699999999</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1367,14 +1377,15 @@
         <v>39</v>
       </c>
       <c r="D4" s="12">
-        <v>-426.63560000000143</v>
-      </c>
-      <c r="E4" s="12">
+        <f>O_TransactionActivity2!G4</f>
+        <v>-436.00540000000001</v>
+      </c>
+      <c r="E4" s="14">
         <f>F3</f>
-        <v>16127.9249</v>
-      </c>
-      <c r="F4" s="12">
-        <f>E4+D4</f>
+        <v>16137.294699999999</v>
+      </c>
+      <c r="F4" s="15">
+        <f>D4+E4</f>
         <v>15701.289299999999</v>
       </c>
     </row>
@@ -1393,7 +1404,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1522,7 +1533,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1592,7 +1603,7 @@
         <v>43</v>
       </c>
       <c r="G3">
-        <v>437.89499999999998</v>
+        <v>438.15229999999997</v>
       </c>
       <c r="H3" s="7">
         <v>202409</v>
@@ -1624,7 +1635,7 @@
         <v>43</v>
       </c>
       <c r="G4" s="11">
-        <v>-73.215900000000033</v>
+        <v>-73.47320000000002</v>
       </c>
       <c r="H4" s="7">
         <v>202412</v>
@@ -1651,7 +1662,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1721,7 +1732,7 @@
         <v>46</v>
       </c>
       <c r="G3">
-        <v>437854.35</v>
+        <v>437854.35000000003</v>
       </c>
       <c r="H3" s="7">
         <v>202409</v>
@@ -1753,7 +1764,7 @@
         <v>46</v>
       </c>
       <c r="G4" s="8">
-        <v>-5671.234999999986</v>
+        <v>-5671.2350000000442</v>
       </c>
       <c r="H4" s="7">
         <v>202412</v>
@@ -1780,7 +1791,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1831,13 +1842,14 @@
         <v>41</v>
       </c>
       <c r="D3" s="12">
+        <f>O_TransactionActivity3!G3</f>
         <v>945.57389999999998</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="9">
         <v>0</v>
       </c>
-      <c r="F3" s="12">
-        <f>D3</f>
+      <c r="F3" s="15">
+        <f>D3+E3</f>
         <v>945.57389999999998</v>
       </c>
     </row>
@@ -1852,14 +1864,15 @@
         <v>41</v>
       </c>
       <c r="D4" s="12">
+        <f>O_TransactionActivity3!G4</f>
         <v>-537.53749999999991</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="14">
         <f>F3</f>
         <v>945.57389999999998</v>
       </c>
-      <c r="F4" s="12">
-        <f>E4+D4</f>
+      <c r="F4" s="15">
+        <f>D4+E4</f>
         <v>408.03640000000007</v>
       </c>
     </row>

</xml_diff>